<commit_message>
finish weight to bmi transform
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djaimes/running/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE25BD9A-77BF-904D-93BA-B3998B37FAAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A1DA93-4F0C-C045-A32F-C216DEC23443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27940" windowHeight="17540" activeTab="1" xr2:uid="{7422E182-634F-324C-A23E-459F39EC114B}"/>
   </bookViews>
@@ -48,10 +48,10 @@
     <t>Weight (lbs)</t>
   </si>
   <si>
-    <t>BMI</t>
+    <t>weight</t>
   </si>
   <si>
-    <t>Weight (ibs)</t>
+    <t>bmi</t>
   </si>
 </sst>
 </file>
@@ -488,17 +488,17 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>